<commit_message>
Updated experiment salinity split 2016-17/18-19 - updated dataset - in 'run_experiment_training_2016_2017_test_2018_2019.m' computed old model metrics on 2018 / 2019
</commit_message>
<xml_diff>
--- a/Parameters-Estimation/Salinity_Estimation/1-Trained-Models/training_2016_2017_test_2018_2019_comparing_old_model/Results-salinity-calibration-model-k-10-old-configuration.xlsx
+++ b/Parameters-Estimation/Salinity_Estimation/1-Trained-Models/training_2016_2017_test_2018_2019_comparing_old_model/Results-salinity-calibration-model-k-10-old-configuration.xlsx
@@ -13,7 +13,46 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>Row</t>
+  </si>
+  <si>
+    <t>random_forest</t>
+  </si>
+  <si>
+    <t>lsboost</t>
+  </si>
+  <si>
+    <t>neural_network</t>
+  </si>
+  <si>
+    <t>old_model</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>NRMSE</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>RSE</t>
+  </si>
+  <si>
+    <t>RRSE</t>
+  </si>
+  <si>
+    <t>RAE</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Corr Coeff</t>
+  </si>
   <si>
     <t>Row</t>
   </si>
@@ -113,123 +152,123 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0">
-        <v>3.6735875436719931</v>
+        <v>3.6568046469664277</v>
       </c>
       <c r="C2" s="0">
-        <v>0.23037650029494589</v>
+        <v>0.22932401822887949</v>
       </c>
       <c r="D2" s="0">
-        <v>2.772327960590848</v>
+        <v>2.7551307925967832</v>
       </c>
       <c r="E2" s="0">
-        <v>0.38637855834058044</v>
+        <v>0.38285625817950447</v>
       </c>
       <c r="F2" s="0">
-        <v>0.62159356362544527</v>
+        <v>0.61875379447685364</v>
       </c>
       <c r="G2" s="0">
-        <v>0.57985787936239719</v>
+        <v>0.57626093358042985</v>
       </c>
       <c r="H2" s="0">
-        <v>0.61362144165941956</v>
+        <v>0.61714374182049547</v>
       </c>
       <c r="I2" s="0">
-        <v>0.78339321987009058</v>
+        <v>0.78566140842942933</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0">
-        <v>3.7317831142344802</v>
+        <v>3.6487532235597304</v>
       </c>
       <c r="C3" s="0">
-        <v>0.23402603680917641</v>
+        <v>0.22881910069941352</v>
       </c>
       <c r="D3" s="0">
-        <v>2.8669919335369896</v>
+        <v>2.7624820257014844</v>
       </c>
       <c r="E3" s="0">
-        <v>0.39871724574122741</v>
+        <v>0.38117219538465258</v>
       </c>
       <c r="F3" s="0">
-        <v>0.63144061141268659</v>
+        <v>0.61739144421076375</v>
       </c>
       <c r="G3" s="0">
-        <v>0.5996577195634355</v>
+        <v>0.57779851156520856</v>
       </c>
       <c r="H3" s="0">
-        <v>0.60128275425877264</v>
+        <v>0.61882780461534748</v>
       </c>
       <c r="I3" s="0">
-        <v>0.77552536386939064</v>
+        <v>0.78704235753092244</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0">
-        <v>3.8888903942891573</v>
+        <v>3.8032154909667311</v>
       </c>
       <c r="C4" s="0">
-        <v>0.24387848347597788</v>
+        <v>0.23850567442872173</v>
       </c>
       <c r="D4" s="0">
-        <v>2.9316082954892382</v>
+        <v>2.8551359709596573</v>
       </c>
       <c r="E4" s="0">
-        <v>0.43299575255675082</v>
+        <v>0.41412752492609234</v>
       </c>
       <c r="F4" s="0">
-        <v>0.65802412764027951</v>
+        <v>0.64352740806129805</v>
       </c>
       <c r="G4" s="0">
-        <v>0.61317282569314413</v>
+        <v>0.59717793599683799</v>
       </c>
       <c r="H4" s="0">
-        <v>0.56700424744324918</v>
+        <v>0.58587247507390772</v>
       </c>
       <c r="I4" s="0">
-        <v>0.75442388094282986</v>
+        <v>0.76549544100335287</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0">
         <v>6.6458686365368624</v>

</xml_diff>